<commit_message>
Updated 2HPico DSP schematic, BOM and JLCPCB assy files
BOM changes as a result of further testing: R1 -> 47 ohms, R10,R17->10k.
</commit_message>
<xml_diff>
--- a/2HPico DSP KiCad Design Files/Pico 2HP_Audio/Pico 2HP_Audio_BOM.xlsx
+++ b/2HPico DSP KiCad Design Files/Pico 2HP_Audio/Pico 2HP_Audio_BOM.xlsx
@@ -103,9 +103,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>100R</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>most 22u SMT caps will fit on the pads</t>
+  </si>
+  <si>
+    <t>47R</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1237,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,10 +1264,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1281,10 +1281,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1298,13 +1298,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -1321,7 +1321,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1338,7 +1338,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1355,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1372,7 +1372,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>
@@ -1389,7 +1389,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s">
         <v>18</v>
@@ -1406,10 +1406,10 @@
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
@@ -1423,13 +1423,13 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
         <v>6</v>
@@ -1446,10 +1446,10 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
@@ -1466,10 +1466,10 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
         <v>6</v>
@@ -1486,7 +1486,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
         <v>6</v>
@@ -1500,10 +1500,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
@@ -1511,16 +1511,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -1528,16 +1528,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
         <v>6</v>
@@ -1545,16 +1545,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
         <v>6</v>
@@ -1562,16 +1562,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -1579,16 +1579,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
         <v>6</v>
@@ -1596,16 +1596,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G20" t="s">
         <v>6</v>
@@ -1613,16 +1613,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G21" t="s">
         <v>6</v>
@@ -1630,16 +1630,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" t="s">
         <v>6</v>
@@ -1647,16 +1647,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
         <v>6</v>
@@ -1664,16 +1664,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
         <v>6</v>
@@ -1681,159 +1681,159 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
       <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" t="s">
         <v>51</v>
-      </c>
-      <c r="D26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>82</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" t="s">
         <v>54</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" t="s">
-        <v>93</v>
-      </c>
-      <c r="G27" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" t="s">
         <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" t="s">
-        <v>92</v>
-      </c>
-      <c r="G28" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" t="s">
         <v>60</v>
-      </c>
-      <c r="D29" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" t="s">
         <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E30" t="s">
-        <v>95</v>
-      </c>
-      <c r="G30" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" t="s">
         <v>66</v>
-      </c>
-      <c r="D31" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>